<commit_message>
added r script for processing csv
</commit_message>
<xml_diff>
--- a/Files/Other/Subject Biographic Info.xlsx
+++ b/Files/Other/Subject Biographic Info.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sf1\Users\faculty\derya\My Documents\research\Ioannis\FacialExpressionsData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Personal\Driving\Files\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10200"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,6 @@
     <t>T088</t>
   </si>
   <si>
-    <t>Age (Y Young, O Old)</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -246,12 +243,15 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -589,16 +589,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -609,10 +614,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,10 +625,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,10 +636,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,10 +647,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,10 +658,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,10 +669,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,10 +680,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,10 +691,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,10 +713,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +724,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,10 +735,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -741,10 +746,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,10 +757,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,10 +768,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,10 +779,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,10 +790,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,10 +801,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,10 +812,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,10 +823,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,10 +834,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,10 +845,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,10 +856,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,10 +867,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,10 +878,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,10 +889,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,10 +900,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,10 +911,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,10 +922,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,10 +933,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +944,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +955,10 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,10 +966,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,10 +977,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,10 +988,10 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,10 +999,10 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,10 +1010,10 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,10 +1021,10 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1032,10 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,10 +1043,10 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,10 +1054,10 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,10 +1065,10 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,10 +1076,10 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,10 +1087,10 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,10 +1098,10 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1104,10 +1109,10 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1115,10 +1120,10 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,10 +1131,10 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,10 +1142,10 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,10 +1153,10 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1164,10 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,10 +1175,10 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1186,10 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,10 +1197,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,10 +1208,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,10 +1219,10 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1230,10 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,10 +1241,10 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,10 +1252,10 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,10 +1263,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,10 +1274,10 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,10 +1285,10 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1296,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,10 +1307,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,10 +1318,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,10 +1329,10 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,10 +1340,10 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,10 +1351,10 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>